<commit_message>
Small contributions, updates, and edits to White Paper.
</commit_message>
<xml_diff>
--- a/docs/whitepaper/src/Summary_Eng-Tech_Table.xlsx
+++ b/docs/whitepaper/src/Summary_Eng-Tech_Table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jg/development/scala/visionav/docs/whitepaper/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jg/development/scala/vision/docs/whitepaper/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="66620" yWindow="460" windowWidth="22340" windowHeight="23140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -532,7 +532,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Additions to White Paper, bibliography
</commit_message>
<xml_diff>
--- a/docs/whitepaper/src/Summary_Eng-Tech_Table.xlsx
+++ b/docs/whitepaper/src/Summary_Eng-Tech_Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="66620" yWindow="460" windowWidth="22340" windowHeight="23140" tabRatio="500"/>
+    <workbookView xWindow="44240" yWindow="460" windowWidth="22340" windowHeight="23140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>Client Devices</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
     <t>subtopic</t>
   </si>
   <si>
@@ -196,7 +193,10 @@
     <t>Hardware, Vendor Implementations</t>
   </si>
   <si>
-    <t>DisplayPort, IEEE 1394</t>
+    <t>DisplayPort, IEEE 1394, Decoders</t>
+  </si>
+  <si>
+    <t>domain</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,13 +544,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -576,7 +576,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -589,53 +589,53 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -643,43 +643,43 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>